<commit_message>
Updated parameters, major improvement
</commit_message>
<xml_diff>
--- a/Graphs/CI Results.xlsx
+++ b/Graphs/CI Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\David\Documents\Work\University\Year 4\Computational Intelligence\CI_Coursework\Graphs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92285969-8A44-4C19-85BB-C8D6A76E169C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96154FCC-1E18-4757-837D-2E29BA4BD3B0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21924" yWindow="3516" windowWidth="7176" windowHeight="7104" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11136" yWindow="2664" windowWidth="7500" windowHeight="7104" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,49 +18,43 @@
   <definedNames>
     <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$B$3:$B$12</definedName>
     <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$C$3:$C$12</definedName>
-    <definedName name="_xlchart.v1.10" hidden="1">Sheet1!$B$45:$B$49</definedName>
-    <definedName name="_xlchart.v1.11" hidden="1">Sheet1!$C$37:$C$41</definedName>
-    <definedName name="_xlchart.v1.12" hidden="1">Sheet1!$C$45:$C$49</definedName>
-    <definedName name="_xlchart.v1.13" hidden="1">Sheet1!$D$37:$D$41</definedName>
-    <definedName name="_xlchart.v1.14" hidden="1">Sheet1!$D$45:$D$49</definedName>
-    <definedName name="_xlchart.v1.15" hidden="1">Sheet1!$B$16</definedName>
-    <definedName name="_xlchart.v1.16" hidden="1">Sheet1!$B$16:$B$25</definedName>
-    <definedName name="_xlchart.v1.17" hidden="1">Sheet1!$B$17:$B$25</definedName>
-    <definedName name="_xlchart.v1.18" hidden="1">Sheet1!$B$3:$B$12</definedName>
-    <definedName name="_xlchart.v1.19" hidden="1">Sheet1!$C$16:$C$25</definedName>
+    <definedName name="_xlchart.v1.10" hidden="1">Sheet1!$C$37:$C$41</definedName>
+    <definedName name="_xlchart.v1.11" hidden="1">Sheet1!$D$37:$D$41</definedName>
+    <definedName name="_xlchart.v1.12" hidden="1">Sheet1!$B$16:$B$25</definedName>
+    <definedName name="_xlchart.v1.13" hidden="1">Sheet1!$C$16:$C$25</definedName>
+    <definedName name="_xlchart.v1.14" hidden="1">Sheet1!$D$16:$D$25</definedName>
+    <definedName name="_xlchart.v1.15" hidden="1">Sheet1!$B$53:$B$62</definedName>
+    <definedName name="_xlchart.v1.16" hidden="1">Sheet1!$C$53:$C$62</definedName>
+    <definedName name="_xlchart.v1.17" hidden="1">Sheet1!$D$53:$D$62</definedName>
+    <definedName name="_xlchart.v1.18" hidden="1">Sheet1!$B$53:$B$62</definedName>
+    <definedName name="_xlchart.v1.19" hidden="1">Sheet1!$B$66:$B$75</definedName>
     <definedName name="_xlchart.v1.2" hidden="1">Sheet1!$D$3:$D$12</definedName>
-    <definedName name="_xlchart.v1.20" hidden="1">Sheet1!$C$3:$C$12</definedName>
-    <definedName name="_xlchart.v1.21" hidden="1">Sheet1!$D$16:$D$25</definedName>
-    <definedName name="_xlchart.v1.22" hidden="1">Sheet1!$D$3:$D$12</definedName>
-    <definedName name="_xlchart.v1.23" hidden="1">Sheet1!$B$16:$B$25</definedName>
-    <definedName name="_xlchart.v1.24" hidden="1">Sheet1!$B$29:$B$33</definedName>
-    <definedName name="_xlchart.v1.25" hidden="1">Sheet1!$C$16:$C$25</definedName>
-    <definedName name="_xlchart.v1.26" hidden="1">Sheet1!$C$29:$C$33</definedName>
-    <definedName name="_xlchart.v1.27" hidden="1">Sheet1!$D$16:$D$25</definedName>
-    <definedName name="_xlchart.v1.28" hidden="1">Sheet1!$D$29:$D$33</definedName>
-    <definedName name="_xlchart.v1.29" hidden="1">Sheet1!$B$29:$B$33</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Sheet1!$B$29:$B$33</definedName>
-    <definedName name="_xlchart.v1.30" hidden="1">Sheet1!$B$53:$B$62</definedName>
-    <definedName name="_xlchart.v1.31" hidden="1">Sheet1!$C$29:$C$33</definedName>
-    <definedName name="_xlchart.v1.32" hidden="1">Sheet1!$C$53:$C$62</definedName>
-    <definedName name="_xlchart.v1.33" hidden="1">Sheet1!$D$29:$D$33</definedName>
-    <definedName name="_xlchart.v1.34" hidden="1">Sheet1!$D$53:$D$62</definedName>
-    <definedName name="_xlchart.v1.35" hidden="1">Sheet1!$B$29:$B$33</definedName>
-    <definedName name="_xlchart.v1.36" hidden="1">Sheet1!$C$29:$C$33</definedName>
-    <definedName name="_xlchart.v1.37" hidden="1">Sheet1!$D$29:$D$33</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">Sheet1!$B$37:$B$41</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">Sheet1!$C$29:$C$33</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">Sheet1!$C$37:$C$41</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">Sheet1!$D$29:$D$33</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">Sheet1!$D$37:$D$41</definedName>
+    <definedName name="_xlchart.v1.20" hidden="1">Sheet1!$C$53:$C$62</definedName>
+    <definedName name="_xlchart.v1.21" hidden="1">Sheet1!$C$66:$C$75</definedName>
+    <definedName name="_xlchart.v1.22" hidden="1">Sheet1!$D$53:$D$62</definedName>
+    <definedName name="_xlchart.v1.23" hidden="1">Sheet1!$D$66:$D$75</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">Sheet1!$B$45:$B$49</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">Sheet1!$C$45:$C$49</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">Sheet1!$D$45:$D$49</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">Sheet1!$B$29:$B$33</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">Sheet1!$C$29:$C$33</definedName>
+    <definedName name="_xlchart.v1.8" hidden="1">Sheet1!$D$29:$D$33</definedName>
     <definedName name="_xlchart.v1.9" hidden="1">Sheet1!$B$37:$B$41</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="20">
   <si>
     <t>Run/Solution</t>
   </si>
@@ -194,6 +188,12 @@
       <t xml:space="preserve"> worst mutation regardless of mutation rate</t>
     </r>
   </si>
+  <si>
+    <t>Solution Four</t>
+  </si>
+  <si>
+    <t>mutationRate: 0.2, mutationChange: 0.2</t>
+  </si>
 </sst>
 </file>
 
@@ -228,7 +228,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -259,6 +259,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -272,14 +278,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -287,6 +290,10 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -364,6 +371,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{D64F9514-1DCE-4D67-B3A0-74CE0DF060A2}" formatIdx="0">
           <cx:tx>
             <cx:txData>
+              <cx:f/>
               <cx:v>Average Fitness</cx:v>
             </cx:txData>
           </cx:tx>
@@ -375,6 +383,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{00000002-F2BE-4ACC-A4BF-2F1713455376}">
           <cx:tx>
             <cx:txData>
+              <cx:f/>
               <cx:v>Best Fitness</cx:v>
             </cx:txData>
           </cx:tx>
@@ -386,6 +395,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{00000003-F2BE-4ACC-A4BF-2F1713455376}">
           <cx:tx>
             <cx:txData>
+              <cx:f/>
               <cx:v>Fitness with test</cx:v>
             </cx:txData>
           </cx:tx>
@@ -444,17 +454,17 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.16</cx:f>
+        <cx:f>_xlchart.v1.12</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="1">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.19</cx:f>
+        <cx:f>_xlchart.v1.13</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="2">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.21</cx:f>
+        <cx:f>_xlchart.v1.14</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -492,6 +502,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{E16ED8FD-3D0D-4AD6-B646-C2A3222557A4}">
           <cx:tx>
             <cx:txData>
+              <cx:f/>
               <cx:v>Average fitness</cx:v>
             </cx:txData>
           </cx:tx>
@@ -503,6 +514,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{00000001-7DE5-4B0F-934F-FA529E35CBDF}">
           <cx:tx>
             <cx:txData>
+              <cx:f/>
               <cx:v>Best Fitness</cx:v>
             </cx:txData>
           </cx:tx>
@@ -514,6 +526,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{00000002-7DE5-4B0F-934F-FA529E35CBDF}">
           <cx:tx>
             <cx:txData>
+              <cx:f/>
               <cx:v>Fitness with test</cx:v>
             </cx:txData>
           </cx:tx>
@@ -572,17 +585,17 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.24</cx:f>
+        <cx:f>_xlchart.v1.6</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="1">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.26</cx:f>
+        <cx:f>_xlchart.v1.7</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="2">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.28</cx:f>
+        <cx:f>_xlchart.v1.8</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -703,17 +716,17 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.4</cx:f>
+        <cx:f>_xlchart.v1.9</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="1">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.6</cx:f>
+        <cx:f>_xlchart.v1.10</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="2">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.8</cx:f>
+        <cx:f>_xlchart.v1.11</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -834,17 +847,17 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.10</cx:f>
+        <cx:f>_xlchart.v1.3</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="1">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.12</cx:f>
+        <cx:f>_xlchart.v1.4</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="2">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.14</cx:f>
+        <cx:f>_xlchart.v1.5</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -966,17 +979,17 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.30</cx:f>
+        <cx:f>_xlchart.v1.15</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="1">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.32</cx:f>
+        <cx:f>_xlchart.v1.16</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="2">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.34</cx:f>
+        <cx:f>_xlchart.v1.17</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -1005,6 +1018,137 @@
               <a:latin typeface="Calibri" panose="020F0502020204030204"/>
             </a:rPr>
             <a:t>Solution Three Spread of Results</a:t>
+          </a:r>
+        </a:p>
+      </cx:txPr>
+    </cx:title>
+    <cx:plotArea>
+      <cx:plotAreaRegion>
+        <cx:series layoutId="boxWhisker" uniqueId="{E16ED8FD-3D0D-4AD6-B646-C2A3222557A4}">
+          <cx:tx>
+            <cx:txData>
+              <cx:f/>
+              <cx:v>Average fitness</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:dataId val="0"/>
+          <cx:layoutPr>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+        <cx:series layoutId="boxWhisker" uniqueId="{00000001-7DE5-4B0F-934F-FA529E35CBDF}">
+          <cx:tx>
+            <cx:txData>
+              <cx:f/>
+              <cx:v>Best Fitness</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:dataId val="1"/>
+          <cx:layoutPr>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+        <cx:series layoutId="boxWhisker" uniqueId="{00000002-7DE5-4B0F-934F-FA529E35CBDF}">
+          <cx:tx>
+            <cx:txData>
+              <cx:f/>
+              <cx:v>Fitness with test</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:dataId val="2"/>
+          <cx:layoutPr>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+      </cx:plotAreaRegion>
+      <cx:axis id="0" hidden="1">
+        <cx:catScaling gapWidth="1.10000002"/>
+        <cx:tickLabels/>
+      </cx:axis>
+      <cx:axis id="1">
+        <cx:valScaling/>
+        <cx:title>
+          <cx:tx>
+            <cx:txData>
+              <cx:v>Fitness</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:txPr>
+            <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="ctr" rtl="0">
+                <a:defRPr/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="en-US" sz="900" b="1" i="0" u="none" strike="noStrike" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:sysClr>
+                  </a:solidFill>
+                  <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+                </a:rPr>
+                <a:t>Fitness</a:t>
+              </a:r>
+            </a:p>
+          </cx:txPr>
+        </cx:title>
+        <cx:majorGridlines/>
+        <cx:tickLabels/>
+        <cx:numFmt formatCode="0.00" sourceLinked="0"/>
+      </cx:axis>
+    </cx:plotArea>
+    <cx:legend pos="t" align="ctr" overlay="0"/>
+  </cx:chart>
+</cx:chartSpace>
+</file>
+
+<file path=xl/charts/chartEx7.xml><?xml version="1.0" encoding="utf-8"?>
+<cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
+  <cx:chartData>
+    <cx:data id="0">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.19</cx:f>
+      </cx:numDim>
+    </cx:data>
+    <cx:data id="1">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.21</cx:f>
+      </cx:numDim>
+    </cx:data>
+    <cx:data id="2">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.23</cx:f>
+      </cx:numDim>
+    </cx:data>
+  </cx:chartData>
+  <cx:chart>
+    <cx:title pos="t" align="ctr" overlay="0">
+      <cx:tx>
+        <cx:txData>
+          <cx:v>Solution Four Spread of Results</cx:v>
+        </cx:txData>
+      </cx:tx>
+      <cx:txPr>
+        <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1800" b="1" i="0" u="none" strike="noStrike" cap="all" spc="150" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
+                </a:sysClr>
+              </a:solidFill>
+              <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+            </a:rPr>
+            <a:t>Solution Four Spread of Results</a:t>
           </a:r>
         </a:p>
       </cx:txPr>
@@ -1332,6 +1476,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="407">
   <cs:axisTitle>
@@ -3903,6 +4087,520 @@
 </file>
 
 <file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="407">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:effectLst>
+        <a:innerShdw blurRad="114300">
+          <a:schemeClr val="phClr"/>
+        </a:innerShdw>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+            <a:lumOff val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat">
+        <a:solidFill>
+          <a:srgbClr val="D9D9D9"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1800" b="1" cap="all" spc="150"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="407">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -4468,8 +5166,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="6165850" y="0"/>
-              <a:ext cx="4705350" cy="2400300"/>
+              <a:off x="6135370" y="0"/>
+              <a:ext cx="4705350" cy="2749550"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -4549,8 +5247,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="6159500" y="2781300"/>
-              <a:ext cx="4705350" cy="2768600"/>
+              <a:off x="6129020" y="2762250"/>
+              <a:ext cx="4705350" cy="2749550"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -4630,8 +5328,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="6191250" y="5562600"/>
-              <a:ext cx="4705350" cy="2768600"/>
+              <a:off x="6122670" y="5524500"/>
+              <a:ext cx="4705350" cy="2749550"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -4711,8 +5409,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="10896600" y="5562600"/>
-              <a:ext cx="4705350" cy="2768600"/>
+              <a:off x="10828020" y="5524500"/>
+              <a:ext cx="4705350" cy="2749550"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -4792,8 +5490,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="15963900" y="5708650"/>
-              <a:ext cx="4705350" cy="2768600"/>
+              <a:off x="15895320" y="5669280"/>
+              <a:ext cx="4705350" cy="2749550"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -4873,8 +5571,89 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="6210300" y="9391650"/>
-              <a:ext cx="4705350" cy="2768600"/>
+              <a:off x="6141720" y="9326880"/>
+              <a:ext cx="4705350" cy="2749550"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-GB" sz="1100"/>
+                <a:t>This chart isn't available in your version of Excel.
+Editing this shape or saving this workbook into a different file format will permanently break the chart.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>7620</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>445770</xdr:colOff>
+      <xdr:row>81</xdr:row>
+      <xdr:rowOff>13970</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="8" name="Chart 7">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1E6A5EDB-DF8D-4B21-B40D-BBE5FDF72E93}"/>
+                </a:ext>
+                <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+                  <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{4A2CDC83-5AA0-4D65-8E3D-861C7B5BE825}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2014/chartex">
+              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="6149340" y="12077700"/>
+              <a:ext cx="4705350" cy="2749550"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -5490,21 +6269,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H64"/>
+  <dimension ref="A1:H77"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
+      <selection activeCell="E72" sqref="E72"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.36328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.26953125" customWidth="1"/>
-    <col min="3" max="3" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.21875" customWidth="1"/>
+    <col min="3" max="3" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5518,21 +6297,21 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -5546,7 +6325,7 @@
         <v>0.258081383</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>2</v>
       </c>
@@ -5560,7 +6339,7 @@
         <v>1.7754965000000001E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>3</v>
       </c>
@@ -5574,7 +6353,7 @@
         <v>3.5088488000000001E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>4</v>
       </c>
@@ -5588,7 +6367,7 @@
         <v>1.9361095926364001E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>5</v>
       </c>
@@ -5602,7 +6381,7 @@
         <v>0.182122002239551</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>6</v>
       </c>
@@ -5616,7 +6395,7 @@
         <v>0.21956106705862799</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>7</v>
       </c>
@@ -5630,7 +6409,7 @@
         <v>2.05437106432169E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>8</v>
       </c>
@@ -5644,7 +6423,7 @@
         <v>3.5884758438941601E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>9</v>
       </c>
@@ -5658,7 +6437,7 @@
         <v>0.105620024499019</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>10</v>
       </c>
@@ -5672,8 +6451,8 @@
         <v>0.22500339022426399</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A13" s="4" t="s">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B13">
@@ -5689,8 +6468,8 @@
         <v>0.24032641799999999</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A14" s="4" t="s">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B14">
@@ -5706,21 +6485,21 @@
         <v>0.11190208850299843</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>1</v>
       </c>
@@ -5734,7 +6513,7 @@
         <v>3.6587929357620202E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>2</v>
       </c>
@@ -5748,7 +6527,7 @@
         <v>8.9452558006937702E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <v>3</v>
       </c>
@@ -5762,7 +6541,7 @@
         <v>0.22475083704545601</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <v>4</v>
       </c>
@@ -5776,7 +6555,7 @@
         <v>0.10692616109566599</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
         <v>5</v>
       </c>
@@ -5790,7 +6569,7 @@
         <v>0.14381442696177699</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
         <v>6</v>
       </c>
@@ -5804,7 +6583,7 @@
         <v>0.22739851125827201</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
         <v>7</v>
       </c>
@@ -5818,7 +6597,7 @@
         <v>0.21197199247901899</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
         <v>8</v>
       </c>
@@ -5832,7 +6611,7 @@
         <v>2.50505970888425E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
         <v>9</v>
       </c>
@@ -5846,7 +6625,7 @@
         <v>0.208346109077163</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
         <v>10</v>
       </c>
@@ -5860,8 +6639,8 @@
         <v>3.7528336063972198E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A26" s="4" t="s">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A26" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B26">
@@ -5877,8 +6656,8 @@
         <v>0.20234791416942952</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A27" s="4" t="s">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A27" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B27">
@@ -5894,21 +6673,21 @@
         <v>0.13118274584347259</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B28" s="5" t="s">
+      <c r="B28" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C28" s="3"/>
-      <c r="D28" s="3"/>
-      <c r="E28" s="3"/>
-      <c r="F28" s="3"/>
-      <c r="G28" s="3"/>
-      <c r="H28" s="3"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="5"/>
+      <c r="F28" s="5"/>
+      <c r="G28" s="5"/>
+      <c r="H28" s="5"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" s="2">
         <v>1</v>
       </c>
@@ -5922,7 +6701,7 @@
         <v>0.18478160172861399</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" s="2">
         <v>2</v>
       </c>
@@ -5936,7 +6715,7 @@
         <v>0.15389529186321299</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" s="2">
         <v>3</v>
       </c>
@@ -5950,7 +6729,7 @@
         <v>2.94814101741687E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" s="2">
         <v>4</v>
       </c>
@@ -5964,7 +6743,7 @@
         <v>0.22680948186174199</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" s="2">
         <v>5</v>
       </c>
@@ -5978,8 +6757,8 @@
         <v>1.5006457412309099E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A34" s="4" t="s">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A34" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B34">
@@ -5995,8 +6774,8 @@
         <v>0.21180302444943289</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A35" s="4" t="s">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A35" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B35">
@@ -6012,21 +6791,21 @@
         <v>0.12199484860800935</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B36" s="3" t="s">
+      <c r="B36" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C36" s="3"/>
-      <c r="D36" s="3"/>
-      <c r="E36" s="3"/>
-      <c r="F36" s="3"/>
-      <c r="G36" s="3"/>
-      <c r="H36" s="3"/>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="C36" s="5"/>
+      <c r="D36" s="5"/>
+      <c r="E36" s="5"/>
+      <c r="F36" s="5"/>
+      <c r="G36" s="5"/>
+      <c r="H36" s="5"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37" s="2">
         <v>1</v>
       </c>
@@ -6040,7 +6819,7 @@
         <v>0.203330091271957</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38" s="2">
         <v>2</v>
       </c>
@@ -6054,7 +6833,7 @@
         <v>5.5933870942021902E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39" s="2">
         <v>3</v>
       </c>
@@ -6068,7 +6847,7 @@
         <v>0.102303548820378</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40" s="2">
         <v>4</v>
       </c>
@@ -6082,7 +6861,7 @@
         <v>1.54857088207367E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41" s="2">
         <v>5</v>
       </c>
@@ -6096,8 +6875,8 @@
         <v>0.13462464339334501</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A42" s="4" t="s">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A42" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B42">
@@ -6113,8 +6892,8 @@
         <v>0.18784438245122032</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A43" s="4" t="s">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A43" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B43">
@@ -6130,21 +6909,21 @@
         <v>0.10233557264968773</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B44" s="3" t="s">
+      <c r="B44" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C44" s="3"/>
-      <c r="D44" s="3"/>
-      <c r="E44" s="3"/>
-      <c r="F44" s="3"/>
-      <c r="G44" s="3"/>
-      <c r="H44" s="3"/>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="C44" s="5"/>
+      <c r="D44" s="5"/>
+      <c r="E44" s="5"/>
+      <c r="F44" s="5"/>
+      <c r="G44" s="5"/>
+      <c r="H44" s="5"/>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A45" s="2">
         <v>1</v>
       </c>
@@ -6158,7 +6937,7 @@
         <v>2.7409174649033301E-2</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A46" s="2">
         <v>2</v>
       </c>
@@ -6172,7 +6951,7 @@
         <v>0.17073843938201899</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A47" s="2">
         <v>3</v>
       </c>
@@ -6186,7 +6965,7 @@
         <v>2.8311352666268299E-2</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A48" s="2">
         <v>4</v>
       </c>
@@ -6200,7 +6979,7 @@
         <v>0.208033548595428</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A49" s="2">
         <v>5</v>
       </c>
@@ -6214,8 +6993,8 @@
         <v>2.57631727128626E-2</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A50" s="4" t="s">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A50" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B50">
@@ -6231,8 +7010,8 @@
         <v>0.18227037588256539</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A51" s="4" t="s">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A51" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B51">
@@ -6248,21 +7027,21 @@
         <v>9.205113760112224E-2</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B52" s="5" t="s">
+      <c r="B52" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C52" s="3"/>
-      <c r="D52" s="3"/>
-      <c r="E52" s="3"/>
-      <c r="F52" s="3"/>
-      <c r="G52" s="3"/>
-      <c r="H52" s="3"/>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="C52" s="5"/>
+      <c r="D52" s="5"/>
+      <c r="E52" s="5"/>
+      <c r="F52" s="5"/>
+      <c r="G52" s="5"/>
+      <c r="H52" s="5"/>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A53" s="2">
         <v>1</v>
       </c>
@@ -6276,7 +7055,7 @@
         <v>5.97901298479903E-2</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A54" s="2">
         <v>2</v>
       </c>
@@ -6290,7 +7069,7 @@
         <v>0.14298301227156701</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A55" s="2">
         <v>3</v>
       </c>
@@ -6304,7 +7083,7 @@
         <v>2.5337600980768999E-2</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A56" s="2">
         <v>4</v>
       </c>
@@ -6318,7 +7097,7 @@
         <v>0.189740274913304</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A57" s="2">
         <v>5</v>
       </c>
@@ -6332,7 +7111,7 @@
         <v>0.12758269757760901</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A58" s="2">
         <v>6</v>
       </c>
@@ -6346,7 +7125,7 @@
         <v>0.215405855666677</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A59" s="2">
         <v>7</v>
       </c>
@@ -6360,7 +7139,7 @@
         <v>0.23456960132650601</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A60" s="2">
         <v>8</v>
       </c>
@@ -6374,7 +7153,7 @@
         <v>0.20013855185870699</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A61" s="2">
         <v>9</v>
       </c>
@@ -6388,7 +7167,7 @@
         <v>0.14956770374836401</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A62" s="2">
         <v>10</v>
       </c>
@@ -6402,8 +7181,8 @@
         <v>5.7182943981679599E-2</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A63" s="4" t="s">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A63" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B63">
@@ -6419,8 +7198,8 @@
         <v>0.16440267393253499</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A64" s="4" t="s">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A64" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B64">
@@ -6436,8 +7215,197 @@
         <v>0.10908674311824787</v>
       </c>
     </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A65" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B65" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C65" s="5"/>
+      <c r="D65" s="5"/>
+      <c r="E65" s="5"/>
+      <c r="F65" s="5"/>
+      <c r="G65" s="5"/>
+      <c r="H65" s="5"/>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A66" s="2">
+        <v>1</v>
+      </c>
+      <c r="B66">
+        <v>3.55688127102348E-2</v>
+      </c>
+      <c r="C66">
+        <v>1.59356806622842E-2</v>
+      </c>
+      <c r="D66">
+        <v>3.1763970826889497E-2</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A67" s="2">
+        <v>2</v>
+      </c>
+      <c r="B67">
+        <v>2.9870228448984799E-2</v>
+      </c>
+      <c r="C67">
+        <v>1.8154524663669899E-2</v>
+      </c>
+      <c r="D67">
+        <v>2.3431723674260201E-2</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A68" s="2">
+        <v>3</v>
+      </c>
+      <c r="B68" s="6">
+        <v>0.12670660979019099</v>
+      </c>
+      <c r="C68" s="6">
+        <v>0.123122263973602</v>
+      </c>
+      <c r="D68" s="6">
+        <v>0.33383623612494301</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A69" s="2">
+        <v>4</v>
+      </c>
+      <c r="B69">
+        <v>5.2610569698563397E-2</v>
+      </c>
+      <c r="C69">
+        <v>2.9927838280656201E-2</v>
+      </c>
+      <c r="D69">
+        <v>5.2549836165688299E-2</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A70" s="2">
+        <v>5</v>
+      </c>
+      <c r="B70">
+        <v>4.8253850498523897E-2</v>
+      </c>
+      <c r="C70">
+        <v>2.2454602232282399E-2</v>
+      </c>
+      <c r="D70">
+        <v>9.12330891810373E-2</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A71" s="2">
+        <v>6</v>
+      </c>
+      <c r="B71">
+        <v>2.7969792354723699E-2</v>
+      </c>
+      <c r="C71">
+        <v>1.8096190059391701E-2</v>
+      </c>
+      <c r="D71">
+        <v>3.1091274978609099E-2</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A72" s="2">
+        <v>7</v>
+      </c>
+      <c r="B72">
+        <v>4.8717748209552901E-2</v>
+      </c>
+      <c r="C72">
+        <v>2.3970201770411301E-2</v>
+      </c>
+      <c r="D72">
+        <v>7.3158760687053806E-2</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A73" s="2">
+        <v>8</v>
+      </c>
+      <c r="B73">
+        <v>7.1666728902946605E-2</v>
+      </c>
+      <c r="C73">
+        <v>4.59463773354815E-2</v>
+      </c>
+      <c r="D73">
+        <v>0.133108957719072</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A74" s="2">
+        <v>9</v>
+      </c>
+      <c r="B74">
+        <v>6.80787887940877E-2</v>
+      </c>
+      <c r="C74">
+        <v>4.6473025716781899E-2</v>
+      </c>
+      <c r="D74">
+        <v>0.12939274095081199</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A75" s="2">
+        <v>10</v>
+      </c>
+      <c r="B75">
+        <v>8.2394626703449103E-2</v>
+      </c>
+      <c r="C75">
+        <v>5.7726208050802801E-2</v>
+      </c>
+      <c r="D75">
+        <v>0.145349428603993</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A76" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B76">
+        <f>(MAX(B66:B70)-MIN(B66:B70))</f>
+        <v>9.6836381341206201E-2</v>
+      </c>
+      <c r="C76">
+        <f>(MAX(C66:C70)-MIN(C66:C70))</f>
+        <v>0.10718658331131781</v>
+      </c>
+      <c r="D76">
+        <f>(MAX(D66:D70)-MIN(D66:D70))</f>
+        <v>0.31040451245068279</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A77" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B77">
+        <f>AVERAGE(B66:B70)</f>
+        <v>5.860201422929958E-2</v>
+      </c>
+      <c r="C77">
+        <f>AVERAGE(C66:C70)</f>
+        <v>4.1918981962498943E-2</v>
+      </c>
+      <c r="D77">
+        <f>AVERAGE(D66:D70)</f>
+        <v>0.10656297119456366</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="7">
+    <mergeCell ref="B65:H65"/>
     <mergeCell ref="B52:H52"/>
     <mergeCell ref="B2:H2"/>
     <mergeCell ref="B15:H15"/>

</xml_diff>